<commit_message>
Change utilization to use not_installed and make other model selection better
</commit_message>
<xml_diff>
--- a/app/config/tables/cold_rooms/forms/cold_room_status/cold_room_status.xlsx
+++ b/app/config/tables/cold_rooms/forms/cold_room_status/cold_room_status.xlsx
@@ -9,14 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="37944" windowHeight="19704" tabRatio="500"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="37950" windowHeight="19710" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
     <sheet name="choices" sheetId="2" r:id="rId2"/>
     <sheet name="settings" sheetId="5" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -172,15 +172,6 @@
     <t>No En Uso</t>
   </si>
   <si>
-    <t>in_store_for_allocation</t>
-  </si>
-  <si>
-    <t>In Store For Allocation</t>
-  </si>
-  <si>
-    <t>Almacenado Epsperando asignación</t>
-  </si>
-  <si>
     <t>value</t>
   </si>
   <si>
@@ -350,6 +341,15 @@
   </si>
   <si>
     <t>Estado del Cuarto Frio</t>
+  </si>
+  <si>
+    <t>not_installed</t>
+  </si>
+  <si>
+    <t>Not Installed</t>
+  </si>
+  <si>
+    <t>No Instalado</t>
   </si>
 </sst>
 </file>
@@ -860,27 +860,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="42.77734375" customWidth="1"/>
-    <col min="2" max="3" width="11.33203125" customWidth="1"/>
-    <col min="4" max="4" width="20.44140625" customWidth="1"/>
-    <col min="5" max="5" width="25.21875" customWidth="1"/>
-    <col min="6" max="6" width="24.6640625" customWidth="1"/>
-    <col min="7" max="7" width="29.6640625" customWidth="1"/>
-    <col min="8" max="8" width="30.44140625" customWidth="1"/>
-    <col min="9" max="9" width="41.6640625" customWidth="1"/>
-    <col min="10" max="10" width="34.77734375" customWidth="1"/>
-    <col min="11" max="11" width="9.44140625" customWidth="1"/>
-    <col min="12" max="12" width="6.21875" customWidth="1"/>
-    <col min="13" max="1025" width="11.33203125" customWidth="1"/>
+    <col min="1" max="1" width="42.7109375" customWidth="1"/>
+    <col min="2" max="3" width="11.28515625" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" customWidth="1"/>
+    <col min="5" max="5" width="25.28515625" customWidth="1"/>
+    <col min="6" max="6" width="24.7109375" customWidth="1"/>
+    <col min="7" max="7" width="29.7109375" customWidth="1"/>
+    <col min="8" max="8" width="30.42578125" customWidth="1"/>
+    <col min="9" max="9" width="41.7109375" customWidth="1"/>
+    <col min="10" max="10" width="34.7109375" customWidth="1"/>
+    <col min="11" max="11" width="9.42578125" customWidth="1"/>
+    <col min="12" max="12" width="6.28515625" customWidth="1"/>
+    <col min="13" max="1025" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -927,14 +927,14 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>15</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
         <v>16</v>
       </c>
@@ -957,7 +957,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D4" t="s">
         <v>16</v>
       </c>
@@ -965,22 +965,22 @@
         <v>25</v>
       </c>
       <c r="F4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="G4" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="H4" t="s">
         <v>26</v>
       </c>
       <c r="I4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="J4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D5" t="s">
         <v>16</v>
       </c>
@@ -1003,30 +1003,30 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D6" t="s">
         <v>16</v>
       </c>
       <c r="E6" t="s">
+        <v>62</v>
+      </c>
+      <c r="F6" t="s">
+        <v>63</v>
+      </c>
+      <c r="G6" t="s">
+        <v>64</v>
+      </c>
+      <c r="H6" t="s">
         <v>65</v>
       </c>
-      <c r="F6" t="s">
+      <c r="I6" t="s">
         <v>66</v>
       </c>
-      <c r="G6" t="s">
+      <c r="J6" t="s">
         <v>67</v>
       </c>
-      <c r="H6" t="s">
-        <v>68</v>
-      </c>
-      <c r="I6" t="s">
-        <v>69</v>
-      </c>
-      <c r="J6" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>17</v>
       </c>
@@ -1046,20 +1046,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" customWidth="1"/>
-    <col min="2" max="2" width="25.21875" customWidth="1"/>
-    <col min="3" max="3" width="44.21875" customWidth="1"/>
-    <col min="4" max="4" width="32.21875" customWidth="1"/>
-    <col min="5" max="1025" width="8.6640625" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" customWidth="1"/>
+    <col min="3" max="3" width="44.28515625" customWidth="1"/>
+    <col min="4" max="4" width="32.28515625" customWidth="1"/>
+    <col min="5" max="1025" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -1073,7 +1073,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -1087,24 +1087,24 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>25</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="16.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C4" s="3"/>
     </row>
-    <row r="5" spans="1:4" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -1118,77 +1118,77 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>28</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D6" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="19.05" customHeight="1" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>28</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D7" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>28</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>28</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D9" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>28</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D10" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>28</v>
       </c>
@@ -1199,10 +1199,10 @@
         <v>41</v>
       </c>
       <c r="D11" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -1216,7 +1216,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -1230,23 +1230,23 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>19</v>
       </c>
       <c r="B15" t="s">
-        <v>47</v>
+        <v>104</v>
       </c>
       <c r="C15" t="s">
-        <v>48</v>
+        <v>105</v>
       </c>
       <c r="D15" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B17" t="s">
         <v>40</v>
@@ -1255,49 +1255,49 @@
         <v>41</v>
       </c>
       <c r="D17" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B18" t="s">
+        <v>68</v>
+      </c>
+      <c r="C18" t="s">
         <v>71</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>74</v>
       </c>
-      <c r="D18" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B19" t="s">
+        <v>69</v>
+      </c>
+      <c r="C19" t="s">
         <v>72</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>75</v>
       </c>
-      <c r="D19" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B20" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20" t="s">
         <v>73</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>76</v>
-      </c>
-      <c r="D20" t="s">
-        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1319,20 +1319,20 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
     <col min="2" max="2" width="23" customWidth="1"/>
-    <col min="3" max="3" width="28.33203125" customWidth="1"/>
-    <col min="4" max="1025" width="11.33203125" customWidth="1"/>
+    <col min="3" max="3" width="28.28515625" customWidth="1"/>
+    <col min="4" max="1025" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C1" t="s">
         <v>6</v>
@@ -1341,75 +1341,75 @@
         <v>7</v>
       </c>
       <c r="E1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="F1" t="s">
+      <c r="B3" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>53</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="16.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="16.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="16.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>56</v>
       </c>
       <c r="B4" s="2">
         <v>20191006</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="16.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>56</v>
+      </c>
+      <c r="E7" t="s">
+        <v>57</v>
+      </c>
+      <c r="F7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>59</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E8" t="s">
         <v>60</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F8" t="s">
         <v>61</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>62</v>
-      </c>
-      <c r="E8" t="s">
-        <v>63</v>
-      </c>
-      <c r="F8" t="s">
-        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>